<commit_message>
Recommendation based on interest + data prep
</commit_message>
<xml_diff>
--- a/datasets/users/researchers.xlsx
+++ b/datasets/users/researchers.xlsx
@@ -423,7 +423,7 @@
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="30" customWidth="1" min="2" max="2"/>
-    <col width="498" customWidth="1" min="3" max="3"/>
+    <col width="507" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['Computer Science', 'Engineering', 'Telecommunications', 'Automation &amp; Control Systems']</t>
+          <t>['Computer Science', 'Software Engineering', 'Telecommunications', 'Automation &amp; Control Systems']</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -498,7 +498,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['Natural language processing', 'Machine learning', 'Artificial intelligence', 'Algorithms', 'Logical design', 'Teaching technology-enhanced learning', 'Group knowledge', 'Virtual teams', 'Collaboration']</t>
+          <t>['NLP', 'Machine learning', 'Artificial intelligence', 'Algorithms', 'Logical design', 'Teaching technology-enhanced learning', 'Group knowledge', 'Virtual teams', 'Collaboration']</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -516,7 +516,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['Liquid crystals', 'Liquid crystals, polarised microscopy, magneto-optic and electro-optic properties', 'Carbon based nanomaterials', 'Nanoscience', 'Nanoparticles', 'Magnetic nanomaterials', 'Carbon based nanomaterials', 'Quantum dots', 'Physics', 'Materials Science', 'Mathematics', 'Science &amp; Technology - Other Topics', 'Optics']</t>
+          <t>['Liquid crystal', 'Liquid crystals, polarised microscopy, magneto-optic and electro-optic properties', 'Carbon based nanomaterials', 'Nanoscience', 'Nanoparticles', 'Magnetic nanomaterials', 'Carbon based nanomaterials', 'Quantum dots', 'Physics', 'Materials Science', 'Mathematics', 'Science &amp; Technology - Other Topics', 'Optics']</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -534,7 +534,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['Natural language processing', 'Discourse analysis', 'Learning analytics', 'Artificial intelligence']</t>
+          <t>['NLP', 'Discourse analysis', 'Learning analytics', 'Artificial intelligence']</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -552,7 +552,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>['Computer systems', 'Cyber security']</t>
+          <t>['Systems', 'Security']</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -570,7 +570,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['Communication protocols', 'Distributed systems', 'Mobile apps', 'Internet of things', 'Blockchain', 'Benchmarking', 'IT business models', 'Business Model Canvas', 'Activity plan', 'Gantt', 'Training', 'Digitization', 'Digital skills', 'Social values', 'Competences']</t>
+          <t>['Communication protocols', 'Distributed systems', 'Mobile apps', 'Internet of things', 'Blockchain', 'Benchmark', 'IT business models', 'Business Model Canvas', 'Activity plan', 'Gantt', 'Training', 'Digitization', 'Digital skills', 'Social values', 'Competences']</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -588,7 +588,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>['Artificial intelligence', 'Ambient intelligence', 'Machine learning', 'Social robotics', 'Intelligent agents', 'E-learning', 'Learning analytics', 'Deep learning', 'AI', 'NLP', 'Soft computing', 'Cloud computing']</t>
+          <t>['Artificial intelligence', 'Ambient intelligence', 'Machine learning', 'Social robotics', 'Intelligent agent', 'E-learning', 'Learning analytics', 'Deep learning', 'AI', 'NLP', 'Soft computing', 'Cloud computing']</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -606,7 +606,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>['Distributed Systems', 'BigData', 'Security', 'Communication Protocols']</t>
+          <t>['Distributed Systems', 'Big Data', 'Security', 'Communication Protocols']</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -642,7 +642,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>['Computer Science', 'Engineering', 'Automation &amp; Control Systems', 'Telecommunications', 'Robotics']</t>
+          <t>['Computer Science', 'Software Engineering', 'Automation &amp; Control Systems', 'Telecommunications', 'Robotics']</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -678,7 +678,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>['Information systems', 'Internet of things', 'Cyber physical systems', 'IT infrastructure', 'Computers', 'Networks', 'Internet', 'Systems and communication', 'Systems engineering', 'industry 4.0', 'Smart network', 'Networking', 'Internet', 'Security', 'Robotics', 'Project management', 'Organizational management']</t>
+          <t>['Information system', 'Internet of things', 'Cyber physical system', 'IT infrastructure', 'Computers', 'Networks', 'Internet', 'Systems and communication', 'Systems engineering', 'industry 4.0', 'Smart network', 'Networking', 'Internet', 'Security', 'Robotics', 'Project management', 'Organizational management']</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -714,7 +714,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>['Distributed systems', 'Parallel computing', 'Data structures and algorithms', 'Data science', 'Data analysis', 'Machine learning', 'Computer vision', 'Software engineering', 'Gamification', 'Teaching methods', 'Career development', 'E-learning', 'M-learning']</t>
+          <t>['Distributed systems', 'Parallel computing', 'Data structures', 'Algorithms', 'Data science', 'Data analysis', 'Machine learning', 'Computer vision', 'Software engineering', 'Gamification', 'Teaching methods', 'Career development', 'E-learning', 'M-learning']</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -732,7 +732,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>['Big data', 'Distributed systems', 'Distributed computing', 'Distributed and parallel computing', 'Internet of things', 'Numerical methods', 'Numerical algorithms', 'Numerical estimation', 'Experimental and numerical modelling', 'Optimization', 'Computational physics', 'Numerical modelling', 'Quantum mechanics', 'Relativity', 'Optimization']</t>
+          <t>['Big data', 'Distributed systems', 'Distributed computing', 'parallel computing', 'Internet of things', 'Numerical method', 'Numerical algorithm', 'Numerical estimation', 'Experimental and numerical modelling', 'Optimization', 'Computational physics', 'Numerical modelling', 'Quantum mechanics', 'Relativity', 'Optimization']</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
@@ -750,7 +750,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>['Computer Science', 'Engineering', 'Instruments &amp; Instrumentation', 'Chemistry', 'Telecommunications']</t>
+          <t>['Computer Science', 'Software Engineering', 'Instruments &amp; Instrumentation', 'Chemistry', 'Telecommunications']</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -768,7 +768,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>['IoT', 'IIoT', 'Education', 'Embedded systems', 'Web IoT Programming', 'Computer Science', 'Engineering', 'Instruments &amp; Instrumentation', 'Automation &amp; Control Systems', 'Chemistry']</t>
+          <t>['Internet of Things', 'IoT', 'IIoT', 'Education', 'Embedded systems', 'Web IoT Programming', 'Computer Science', 'Software Engineering', 'Instruments &amp; Instrumentation', 'Automation &amp; Control Systems', 'Chemistry']</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
@@ -804,7 +804,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>['Natural language processing', 'Machine learning', 'Information retrieval', 'Algorithms', 'Artificial intelligence', 'Natural language processing', 'Technology-Enhanced learning']</t>
+          <t>['NLP', 'Machine learning', 'Information retrieval', 'Algorithms', 'Artificial intelligence', 'Technology-Enhanced learning']</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
@@ -822,7 +822,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>['Mobile communications', 'Wireless networks', 'Security and privacy in communications', 'IoT', 'Radio propagation', 'Wearable computing', 'Energy meter', 'Wearable devices']</t>
+          <t>['Mobile communications', 'Wireless networks', 'Security and privacy in communications', 'Internet of Thingd', 'Radio propagation', 'Wearable computing', 'Energy meter', 'Wearable devices']</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
@@ -858,7 +858,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>['Computer Science', 'Education &amp; Educational Research', 'Engineering', 'Linguistics', 'Mathematics']</t>
+          <t>['Computer Science', 'Education &amp; Educational Research', 'Software Engineering', 'Linguistics', 'Mathematics']</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
@@ -876,7 +876,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>['High performance computing', 'Computer systems architecture', 'Automatic differentiation', 'Distributed and parallel computing', 'GPU computing', 'Numerical optimization algorithms', 'Computer modelling and simulation', 'Artificial Intelligence', 'Deep learning', 'Deep Neural Networks', 'Computer Vision', 'Embedded Systems', 'Efficient and scalable parallel algorithms', 'Scientific computing', 'scientific writing', 'Higher education', 'Online courses', 'Domenii ERC 2019', 'Supercomputing']</t>
+          <t>['High performance computing', 'Computer systems architecture', 'Automatic differentiation', 'Distributed computing', 'Parallel computing', 'GPU computing', 'Numerical optimization algorithms', 'Computer modelling and simulation', 'Artificial Intelligence', 'Deep learning', 'Deep Neural Networks', 'Computer Vision', 'Embedded Systems', 'Efficient and scalable parallel algorithms', 'Scientific computing', 'scientific writing', 'Higher education', 'Online courses', 'Domenii ERC 2019', 'Supercomputing']</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -894,7 +894,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>['Computer Science', 'Engineering']</t>
+          <t>['Computer Science', 'Software Engineering']</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
@@ -912,7 +912,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>['Automation &amp; Control Systems', 'Engineering', 'Computer Science', 'Robotics', 'Operations Research &amp; Management Science', 'Diagnosis and fault tolerant control', 'Mixed integer programming', 'Model predictive control', 'Unmanned vehicle systems']</t>
+          <t>['Automation &amp; Control Systems', 'Software Engineering', 'Computer Science', 'Robotics', 'Operations Research &amp; Management Science', 'Diagnosis and fault tolerant control', 'Mixed integer programming', 'Model predictive control', 'Unmanned vehicle systems']</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
@@ -948,7 +948,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>['Business &amp; Economics', 'Engineering', 'Social Sciences - Other Topics', 'Automation &amp; Control Systems', 'Education &amp; Educational Research']</t>
+          <t>['Business &amp; Economics', 'Software Engineering', 'Social Sciences - Other Topics', 'Automation &amp; Control Systems', 'Education &amp; Educational Research']</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
@@ -984,7 +984,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>['Computer Science', 'Engineering', 'Automation &amp; Control Systems', 'Telecommunications', 'Instruments &amp; Instrumentation']</t>
+          <t>['Computer Science', 'Software Engineering', 'Automation &amp; Control Systems', 'Telecommunications', 'Instruments &amp; Instrumentation']</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
@@ -1002,7 +1002,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>['Computer Science', 'Education &amp; Educational Research', 'Engineering', 'Energy &amp; Fuels', 'Automation &amp; Control Systems']</t>
+          <t>['Computer Science', 'Education &amp; Educational Research', 'Software Engineering', 'Energy &amp; Fuels', 'Automation &amp; Control Systems']</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>

</xml_diff>

<commit_message>
common articles + appreciated list
</commit_message>
<xml_diff>
--- a/datasets/users/researchers.xlsx
+++ b/datasets/users/researchers.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -420,30 +432,24 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="30" customWidth="1" min="2" max="2"/>
-    <col width="507" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Researcher ID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Full Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Expertise</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Appreciated</t>
         </is>
@@ -465,7 +471,11 @@
           <t>['Distributed systems', 'IT security', 'Parallel algorithms', 'Machine learning', 'Genetic algorithms']</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>arXiv:2310.02113, arXiv:2310.05269, arXiv:2310.11730, arXiv:2310.09665, arXiv:2310.13424, arXiv:2311.02100, arXiv:2310.01689, arXiv:2310.01676, arXiv:2310.06338, arXiv:2310.04975</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -483,7 +493,11 @@
           <t>['Computer Science', 'Software Engineering', 'Telecommunications', 'Automation &amp; Control Systems']</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>arXiv:2310.03736, arXiv:2310.03702, arXiv:2310.03655, arXiv:2310.03528, arXiv:2310.03501, arXiv:2310.03475, arXiv:2310.03441, arXiv:2310.03178, arXiv:2310.03159, arXiv:2310.03105</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -501,7 +515,11 @@
           <t>['NLP', 'Machine learning', 'Artificial intelligence', 'Algorithms', 'Logical design', 'Teaching technology-enhanced learning', 'Group knowledge', 'Virtual teams', 'Collaboration']</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>arXiv:2310.02357, arXiv:2310.14261, arXiv:2310.01551, arXiv:2310.00526, arXiv:2310.05309, arXiv:2310.19647, arXiv:2311.05511, arXiv:2311.01927, arXiv:2310.04218, arXiv:2310.04425</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -519,7 +537,11 @@
           <t>['Liquid crystal', 'Liquid crystals, polarised microscopy, magneto-optic and electro-optic properties', 'Carbon based nanomaterials', 'Nanoscience', 'Nanoparticles', 'Magnetic nanomaterials', 'Carbon based nanomaterials', 'Quantum dots', 'Physics', 'Materials Science', 'Mathematics', 'Science &amp; Technology - Other Topics', 'Optics']</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>arXiv:2310.04022, arXiv:2310.10524, arXiv:2310.03557, arXiv:2310.03339, arXiv:2310.03254, arXiv:2310.03193, arXiv:2310.01283, arXiv:2310.00394, arXiv:2310.01046, arXiv:2310.00267</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -537,7 +559,11 @@
           <t>['NLP', 'Discourse analysis', 'Learning analytics', 'Artificial intelligence']</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>arXiv:2310.02357, arXiv:2310.00603, arXiv:2310.07086, arXiv:2310.05592, arXiv:2310.09736, arXiv:2310.08977, arXiv:2310.15799, arXiv:2310.14261, arXiv:2311.04925, arXiv:2311.02802</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -555,7 +581,11 @@
           <t>['Systems', 'Security']</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>arXiv:2310.03598, arXiv:2310.03994, arXiv:2310.12254, arXiv:2310.11651, arXiv:2310.10653, arXiv:2310.18820, arXiv:2311.05498, arXiv:2311.05462, arXiv:2311.05037, arXiv:2311.02378</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -573,7 +603,11 @@
           <t>['Communication protocols', 'Distributed systems', 'Mobile apps', 'Internet of things', 'Blockchain', 'Benchmark', 'IT business models', 'Business Model Canvas', 'Activity plan', 'Gantt', 'Training', 'Digitization', 'Digital skills', 'Social values', 'Competences']</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>arXiv:2310.00254, arXiv:2310.04975, arXiv:2310.01689, arXiv:2310.01676, arXiv:2311.02093, arXiv:2310.01594, arXiv:2309.16707, arXiv:2310.07471, arXiv:2310.08822, arXiv:2310.12381</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -591,7 +625,11 @@
           <t>['Artificial intelligence', 'Ambient intelligence', 'Machine learning', 'Social robotics', 'Intelligent agent', 'E-learning', 'Learning analytics', 'Deep learning', 'AI', 'NLP', 'Soft computing', 'Cloud computing']</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>arXiv:2310.01557, arXiv:2310.03086, arXiv:2310.03243, arXiv:2310.02870, arXiv:2310.02422, arXiv:2310.00727, arXiv:2310.00633, arXiv:2310.00010, arXiv:2310.01063, arXiv:2309.16733</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -609,7 +647,11 @@
           <t>['Distributed Systems', 'Big Data', 'Security', 'Communication Protocols']</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>arXiv:2311.00724, arXiv:2311.04517, arXiv:2311.04482, arXiv:2310.02113, arXiv:2310.01689, arXiv:2310.01676, arXiv:2310.06338, arXiv:2310.05269, arXiv:2310.04975, arXiv:2310.03841</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -627,7 +669,11 @@
           <t>['Distributed systems', 'Peer-To-Peer', 'Network security', 'Software engineering']</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>arXiv:2310.08373, arXiv:2310.14283, arXiv:2310.18861, arXiv:2310.09193, arXiv:2310.03618, arXiv:2310.03616, arXiv:2310.02800, arXiv:2310.01893, arXiv:2310.05643, arXiv:2310.12702</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -645,7 +691,11 @@
           <t>['Computer Science', 'Software Engineering', 'Automation &amp; Control Systems', 'Telecommunications', 'Robotics']</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>arXiv:2310.00029, arXiv:2311.02389, arXiv:2310.01039, arXiv:2310.05170, arXiv:2310.15887, arXiv:2311.04569, arXiv:2311.04126, arXiv:2310.03736, arXiv:2310.03702, arXiv:2310.03655</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -663,7 +713,11 @@
           <t>['Image processing', 'Machine learning', 'Ambient intelligence', 'Formal languages', 'Smart environments']</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>arXiv:2310.01003, arXiv:2310.04870, arXiv:2310.03817, arXiv:2310.11678, arXiv:2310.13897, arXiv:2311.00208, arXiv:2311.02433, arXiv:2310.15388, arXiv:2310.10513, arXiv:2311.02460</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -681,7 +735,11 @@
           <t>['Information system', 'Internet of things', 'Cyber physical system', 'IT infrastructure', 'Computers', 'Networks', 'Internet', 'Systems and communication', 'Systems engineering', 'industry 4.0', 'Smart network', 'Networking', 'Internet', 'Security', 'Robotics', 'Project management', 'Organizational management']</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>arXiv:2310.00382, arXiv:2311.04256, arXiv:2310.03401, arXiv:2310.01689, arXiv:2310.01676, arXiv:2310.00254, arXiv:2310.18664, arXiv:2310.18382, arXiv:2310.04975, arXiv:2311.04944</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -699,7 +757,11 @@
           <t>['Distributed systems', 'Distributed data storage', 'Cloud computing', 'Edge computing', 'Resources management']</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>arXiv:2311.00974, arXiv:2310.19013, arXiv:2310.00560, arXiv:2310.06141, arXiv:2310.11957, arXiv:2310.09665, arXiv:2310.16547, arXiv:2311.00271, arXiv:2311.02525, arXiv:2310.03618</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -717,7 +779,11 @@
           <t>['Distributed systems', 'Parallel computing', 'Data structures', 'Algorithms', 'Data science', 'Data analysis', 'Machine learning', 'Computer vision', 'Software engineering', 'Gamification', 'Teaching methods', 'Career development', 'E-learning', 'M-learning']</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>arXiv:2310.00782, arXiv:2309.16682, arXiv:2310.05293, arXiv:2310.15419, arXiv:2310.14977, arXiv:2310.17990, arXiv:2311.04333, arXiv:2311.02811, arXiv:2310.02420, arXiv:2310.08339</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -735,7 +801,11 @@
           <t>['Big data', 'Distributed systems', 'Distributed computing', 'parallel computing', 'Internet of things', 'Numerical method', 'Numerical algorithm', 'Numerical estimation', 'Experimental and numerical modelling', 'Optimization', 'Computational physics', 'Numerical modelling', 'Quantum mechanics', 'Relativity', 'Optimization']</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>arXiv:2311.04517, arXiv:2311.00724, arXiv:2311.04482, arXiv:2310.01689, arXiv:2310.01676, arXiv:2310.00254, arXiv:2310.04975, arXiv:2311.02093, arXiv:2310.08439, arXiv:2310.05701</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -753,7 +823,11 @@
           <t>['Computer Science', 'Software Engineering', 'Instruments &amp; Instrumentation', 'Chemistry', 'Telecommunications']</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>arXiv:2310.03736, arXiv:2310.03702, arXiv:2310.03655, arXiv:2310.03528, arXiv:2310.03501, arXiv:2310.03475, arXiv:2310.03441, arXiv:2310.03178, arXiv:2310.03159, arXiv:2310.03105</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -771,7 +845,11 @@
           <t>['Internet of Things', 'IoT', 'IIoT', 'Education', 'Embedded systems', 'Web IoT Programming', 'Computer Science', 'Software Engineering', 'Instruments &amp; Instrumentation', 'Automation &amp; Control Systems', 'Chemistry']</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>arXiv:2310.18382, arXiv:2310.03401, arXiv:2310.01689, arXiv:2310.01676, arXiv:2310.00254, arXiv:2310.04975, arXiv:2310.18664, arXiv:2311.04944, arXiv:2311.02926, arXiv:2311.02093</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -789,7 +867,11 @@
           <t>['Operator Theory', 'Operator Algebras', 'Functional Analysis', 'Noncommutative Geometry', 'Representation Theory']</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>arXiv:2309.17315, arXiv:2310.00762, arXiv:2310.00290, arXiv:2310.08447, arXiv:2310.10316, arXiv:2310.18078, arXiv:2311.00049, arXiv:2310.19548, arXiv:2310.18565, arXiv:2311.03772</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -807,7 +889,11 @@
           <t>['NLP', 'Machine learning', 'Information retrieval', 'Algorithms', 'Artificial intelligence', 'Technology-Enhanced learning']</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>arXiv:2310.02357, arXiv:2310.14261, arXiv:2310.07874, arXiv:2310.08039, arXiv:2310.04878, arXiv:2310.03919, arXiv:2310.11088, arXiv:2310.16452, arXiv:2310.14079, arXiv:2310.13006</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -825,7 +911,11 @@
           <t>['Mobile communications', 'Wireless networks', 'Security and privacy in communications', 'Internet of Thingd', 'Radio propagation', 'Wearable computing', 'Energy meter', 'Wearable devices']</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>arXiv:2310.00278, arXiv:2310.06857, arXiv:2310.16106, arXiv:2310.16195, arXiv:2310.15705, arXiv:2310.14283, arXiv:2311.05582, arXiv:2310.03744, arXiv:2310.03743, arXiv:2310.03742</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -843,7 +933,11 @@
           <t>['Computer science', 'Tech entrepreneurship', 'Cybersecurity']</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>arXiv:2310.03736, arXiv:2310.03702, arXiv:2310.03655, arXiv:2310.03528, arXiv:2310.03501, arXiv:2310.03475, arXiv:2310.03441, arXiv:2310.03178, arXiv:2310.03159, arXiv:2310.03105</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -861,7 +955,11 @@
           <t>['Computer Science', 'Education &amp; Educational Research', 'Software Engineering', 'Linguistics', 'Mathematics']</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>arXiv:2310.03736, arXiv:2310.03702, arXiv:2310.03655, arXiv:2310.03528, arXiv:2310.03501, arXiv:2310.03475, arXiv:2310.03441, arXiv:2310.03178, arXiv:2310.03159, arXiv:2310.03105</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -879,7 +977,11 @@
           <t>['High performance computing', 'Computer systems architecture', 'Automatic differentiation', 'Distributed computing', 'Parallel computing', 'GPU computing', 'Numerical optimization algorithms', 'Computer modelling and simulation', 'Artificial Intelligence', 'Deep learning', 'Deep Neural Networks', 'Computer Vision', 'Embedded Systems', 'Efficient and scalable parallel algorithms', 'Scientific computing', 'scientific writing', 'Higher education', 'Online courses', 'Domenii ERC 2019', 'Supercomputing']</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>arXiv:2310.02422, arXiv:2311.02840, arXiv:2310.06916, arXiv:2310.04837, arXiv:2310.03294, arXiv:2310.00627, arXiv:2309.16743, arXiv:2310.08401, arXiv:2310.08097, arXiv:2310.07471</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -897,7 +999,11 @@
           <t>['Computer Science', 'Software Engineering']</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>arXiv:2310.03736, arXiv:2310.03702, arXiv:2310.03655, arXiv:2310.03528, arXiv:2310.03501, arXiv:2310.03475, arXiv:2310.03441, arXiv:2310.03178, arXiv:2310.03159, arXiv:2310.03105</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -915,7 +1021,11 @@
           <t>['Automation &amp; Control Systems', 'Software Engineering', 'Computer Science', 'Robotics', 'Operations Research &amp; Management Science', 'Diagnosis and fault tolerant control', 'Mixed integer programming', 'Model predictive control', 'Unmanned vehicle systems']</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>arXiv:2310.01039, arXiv:2310.05170, arXiv:2310.15887, arXiv:2311.04569, arXiv:2311.04126, arXiv:2310.00029, arXiv:2311.02389, arXiv:2310.03673, arXiv:2310.03659, arXiv:2310.03620</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -933,7 +1043,11 @@
           <t>['Computer systems architecture', 'Computer networks', 'Embedded systems', 'Microprocessor systems', 'Distributed systems', 'Internet', 'Mobile computing', 'E-learning', 'Web platforms']</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>arXiv:2310.16214, arXiv:2311.03373, arXiv:2310.04172, arXiv:2311.05063, arXiv:2310.03618, arXiv:2310.03616, arXiv:2310.03568, arXiv:2310.03371, arXiv:2310.03294, arXiv:2310.03200</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -951,7 +1065,11 @@
           <t>['Business &amp; Economics', 'Software Engineering', 'Social Sciences - Other Topics', 'Automation &amp; Control Systems', 'Education &amp; Educational Research']</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>arXiv:2310.03673, arXiv:2310.03659, arXiv:2310.03620, arXiv:2310.03618, arXiv:2310.03616, arXiv:2310.03533, arXiv:2310.03491, arXiv:2310.03318, arXiv:2310.03248, arXiv:2310.03202</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -969,7 +1087,11 @@
           <t>['Databases', 'Data mining', 'Machine learning', 'Text mining']</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>arXiv:2310.05020, arXiv:2310.02540, arXiv:2310.02129, arXiv:2310.01765, arXiv:2310.00749, arXiv:2310.07875, arXiv:2310.07736, arXiv:2310.04830, arXiv:2310.04598, arXiv:2310.04145</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -987,7 +1109,11 @@
           <t>['Computer Science', 'Software Engineering', 'Automation &amp; Control Systems', 'Telecommunications', 'Instruments &amp; Instrumentation']</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>arXiv:2310.03736, arXiv:2310.03702, arXiv:2310.03655, arXiv:2310.03528, arXiv:2310.03501, arXiv:2310.03475, arXiv:2310.03441, arXiv:2310.03178, arXiv:2310.03159, arXiv:2310.03105</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1005,7 +1131,11 @@
           <t>['Computer Science', 'Education &amp; Educational Research', 'Software Engineering', 'Energy &amp; Fuels', 'Automation &amp; Control Systems']</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>arXiv:2310.03736, arXiv:2310.03702, arXiv:2310.03655, arXiv:2310.03528, arXiv:2310.03501, arXiv:2310.03475, arXiv:2310.03441, arXiv:2310.03178, arXiv:2310.03159, arXiv:2310.03105</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
modified import script to modify Authors and Appreciated columns
</commit_message>
<xml_diff>
--- a/datasets/users/researchers.xlsx
+++ b/datasets/users/researchers.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -432,24 +420,30 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="507" customWidth="1" min="3" max="3"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Researcher ID</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Full Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Expertise</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Appreciated</t>
         </is>
@@ -471,11 +465,7 @@
           <t>['Distributed systems', 'IT security', 'Parallel algorithms', 'Machine learning', 'Genetic algorithms']</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>arXiv:2310.02113, arXiv:2310.05269, arXiv:2310.11730, arXiv:2310.09665, arXiv:2310.13424, arXiv:2311.02100, arXiv:2310.01689, arXiv:2310.01676, arXiv:2310.06338, arXiv:2310.04975</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -493,11 +483,7 @@
           <t>['Computer Science', 'Software Engineering', 'Telecommunications', 'Automation &amp; Control Systems']</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>arXiv:2310.03736, arXiv:2310.03702, arXiv:2310.03655, arXiv:2310.03528, arXiv:2310.03501, arXiv:2310.03475, arXiv:2310.03441, arXiv:2310.03178, arXiv:2310.03159, arXiv:2310.03105</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -515,11 +501,7 @@
           <t>['NLP', 'Machine learning', 'Artificial intelligence', 'Algorithms', 'Logical design', 'Teaching technology-enhanced learning', 'Group knowledge', 'Virtual teams', 'Collaboration']</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>arXiv:2310.02357, arXiv:2310.14261, arXiv:2310.01551, arXiv:2310.00526, arXiv:2310.05309, arXiv:2310.19647, arXiv:2311.05511, arXiv:2311.01927, arXiv:2310.04218, arXiv:2310.04425</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -537,11 +519,7 @@
           <t>['Liquid crystal', 'Liquid crystals, polarised microscopy, magneto-optic and electro-optic properties', 'Carbon based nanomaterials', 'Nanoscience', 'Nanoparticles', 'Magnetic nanomaterials', 'Carbon based nanomaterials', 'Quantum dots', 'Physics', 'Materials Science', 'Mathematics', 'Science &amp; Technology - Other Topics', 'Optics']</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>arXiv:2310.04022, arXiv:2310.10524, arXiv:2310.03557, arXiv:2310.03339, arXiv:2310.03254, arXiv:2310.03193, arXiv:2310.01283, arXiv:2310.00394, arXiv:2310.01046, arXiv:2310.00267</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -559,11 +537,7 @@
           <t>['NLP', 'Discourse analysis', 'Learning analytics', 'Artificial intelligence']</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>arXiv:2310.02357, arXiv:2310.00603, arXiv:2310.07086, arXiv:2310.05592, arXiv:2310.09736, arXiv:2310.08977, arXiv:2310.15799, arXiv:2310.14261, arXiv:2311.04925, arXiv:2311.02802</t>
-        </is>
-      </c>
+      <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -581,11 +555,7 @@
           <t>['Systems', 'Security']</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>arXiv:2310.03598, arXiv:2310.03994, arXiv:2310.12254, arXiv:2310.11651, arXiv:2310.10653, arXiv:2310.18820, arXiv:2311.05498, arXiv:2311.05462, arXiv:2311.05037, arXiv:2311.02378</t>
-        </is>
-      </c>
+      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -603,11 +573,7 @@
           <t>['Communication protocols', 'Distributed systems', 'Mobile apps', 'Internet of things', 'Blockchain', 'Benchmark', 'IT business models', 'Business Model Canvas', 'Activity plan', 'Gantt', 'Training', 'Digitization', 'Digital skills', 'Social values', 'Competences']</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>arXiv:2310.00254, arXiv:2310.04975, arXiv:2310.01689, arXiv:2310.01676, arXiv:2311.02093, arXiv:2310.01594, arXiv:2309.16707, arXiv:2310.07471, arXiv:2310.08822, arXiv:2310.12381</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -625,11 +591,7 @@
           <t>['Artificial intelligence', 'Ambient intelligence', 'Machine learning', 'Social robotics', 'Intelligent agent', 'E-learning', 'Learning analytics', 'Deep learning', 'AI', 'NLP', 'Soft computing', 'Cloud computing']</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>arXiv:2310.01557, arXiv:2310.03086, arXiv:2310.03243, arXiv:2310.02870, arXiv:2310.02422, arXiv:2310.00727, arXiv:2310.00633, arXiv:2310.00010, arXiv:2310.01063, arXiv:2309.16733</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -647,11 +609,7 @@
           <t>['Distributed Systems', 'Big Data', 'Security', 'Communication Protocols']</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>arXiv:2311.00724, arXiv:2311.04517, arXiv:2311.04482, arXiv:2310.02113, arXiv:2310.01689, arXiv:2310.01676, arXiv:2310.06338, arXiv:2310.05269, arXiv:2310.04975, arXiv:2310.03841</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -669,11 +627,7 @@
           <t>['Distributed systems', 'Peer-To-Peer', 'Network security', 'Software engineering']</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>arXiv:2310.08373, arXiv:2310.14283, arXiv:2310.18861, arXiv:2310.09193, arXiv:2310.03618, arXiv:2310.03616, arXiv:2310.02800, arXiv:2310.01893, arXiv:2310.05643, arXiv:2310.12702</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -691,11 +645,7 @@
           <t>['Computer Science', 'Software Engineering', 'Automation &amp; Control Systems', 'Telecommunications', 'Robotics']</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>arXiv:2310.00029, arXiv:2311.02389, arXiv:2310.01039, arXiv:2310.05170, arXiv:2310.15887, arXiv:2311.04569, arXiv:2311.04126, arXiv:2310.03736, arXiv:2310.03702, arXiv:2310.03655</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -713,11 +663,7 @@
           <t>['Image processing', 'Machine learning', 'Ambient intelligence', 'Formal languages', 'Smart environments']</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>arXiv:2310.01003, arXiv:2310.04870, arXiv:2310.03817, arXiv:2310.11678, arXiv:2310.13897, arXiv:2311.00208, arXiv:2311.02433, arXiv:2310.15388, arXiv:2310.10513, arXiv:2311.02460</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -735,11 +681,7 @@
           <t>['Information system', 'Internet of things', 'Cyber physical system', 'IT infrastructure', 'Computers', 'Networks', 'Internet', 'Systems and communication', 'Systems engineering', 'industry 4.0', 'Smart network', 'Networking', 'Internet', 'Security', 'Robotics', 'Project management', 'Organizational management']</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>arXiv:2310.00382, arXiv:2311.04256, arXiv:2310.03401, arXiv:2310.01689, arXiv:2310.01676, arXiv:2310.00254, arXiv:2310.18664, arXiv:2310.18382, arXiv:2310.04975, arXiv:2311.04944</t>
-        </is>
-      </c>
+      <c r="D14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -757,11 +699,7 @@
           <t>['Distributed systems', 'Distributed data storage', 'Cloud computing', 'Edge computing', 'Resources management']</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>arXiv:2311.00974, arXiv:2310.19013, arXiv:2310.00560, arXiv:2310.06141, arXiv:2310.11957, arXiv:2310.09665, arXiv:2310.16547, arXiv:2311.00271, arXiv:2311.02525, arXiv:2310.03618</t>
-        </is>
-      </c>
+      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -779,11 +717,7 @@
           <t>['Distributed systems', 'Parallel computing', 'Data structures', 'Algorithms', 'Data science', 'Data analysis', 'Machine learning', 'Computer vision', 'Software engineering', 'Gamification', 'Teaching methods', 'Career development', 'E-learning', 'M-learning']</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>arXiv:2310.00782, arXiv:2309.16682, arXiv:2310.05293, arXiv:2310.15419, arXiv:2310.14977, arXiv:2310.17990, arXiv:2311.04333, arXiv:2311.02811, arXiv:2310.02420, arXiv:2310.08339</t>
-        </is>
-      </c>
+      <c r="D16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -801,11 +735,7 @@
           <t>['Big data', 'Distributed systems', 'Distributed computing', 'parallel computing', 'Internet of things', 'Numerical method', 'Numerical algorithm', 'Numerical estimation', 'Experimental and numerical modelling', 'Optimization', 'Computational physics', 'Numerical modelling', 'Quantum mechanics', 'Relativity', 'Optimization']</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>arXiv:2311.04517, arXiv:2311.00724, arXiv:2311.04482, arXiv:2310.01689, arXiv:2310.01676, arXiv:2310.00254, arXiv:2310.04975, arXiv:2311.02093, arXiv:2310.08439, arXiv:2310.05701</t>
-        </is>
-      </c>
+      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -823,11 +753,7 @@
           <t>['Computer Science', 'Software Engineering', 'Instruments &amp; Instrumentation', 'Chemistry', 'Telecommunications']</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>arXiv:2310.03736, arXiv:2310.03702, arXiv:2310.03655, arXiv:2310.03528, arXiv:2310.03501, arXiv:2310.03475, arXiv:2310.03441, arXiv:2310.03178, arXiv:2310.03159, arXiv:2310.03105</t>
-        </is>
-      </c>
+      <c r="D18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -845,11 +771,7 @@
           <t>['Internet of Things', 'IoT', 'IIoT', 'Education', 'Embedded systems', 'Web IoT Programming', 'Computer Science', 'Software Engineering', 'Instruments &amp; Instrumentation', 'Automation &amp; Control Systems', 'Chemistry']</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>arXiv:2310.18382, arXiv:2310.03401, arXiv:2310.01689, arXiv:2310.01676, arXiv:2310.00254, arXiv:2310.04975, arXiv:2310.18664, arXiv:2311.04944, arXiv:2311.02926, arXiv:2311.02093</t>
-        </is>
-      </c>
+      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -867,11 +789,7 @@
           <t>['Operator Theory', 'Operator Algebras', 'Functional Analysis', 'Noncommutative Geometry', 'Representation Theory']</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>arXiv:2309.17315, arXiv:2310.00762, arXiv:2310.00290, arXiv:2310.08447, arXiv:2310.10316, arXiv:2310.18078, arXiv:2311.00049, arXiv:2310.19548, arXiv:2310.18565, arXiv:2311.03772</t>
-        </is>
-      </c>
+      <c r="D20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -889,11 +807,7 @@
           <t>['NLP', 'Machine learning', 'Information retrieval', 'Algorithms', 'Artificial intelligence', 'Technology-Enhanced learning']</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>arXiv:2310.02357, arXiv:2310.14261, arXiv:2310.07874, arXiv:2310.08039, arXiv:2310.04878, arXiv:2310.03919, arXiv:2310.11088, arXiv:2310.16452, arXiv:2310.14079, arXiv:2310.13006</t>
-        </is>
-      </c>
+      <c r="D21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -911,11 +825,7 @@
           <t>['Mobile communications', 'Wireless networks', 'Security and privacy in communications', 'Internet of Thingd', 'Radio propagation', 'Wearable computing', 'Energy meter', 'Wearable devices']</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>arXiv:2310.00278, arXiv:2310.06857, arXiv:2310.16106, arXiv:2310.16195, arXiv:2310.15705, arXiv:2310.14283, arXiv:2311.05582, arXiv:2310.03744, arXiv:2310.03743, arXiv:2310.03742</t>
-        </is>
-      </c>
+      <c r="D22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -933,11 +843,7 @@
           <t>['Computer science', 'Tech entrepreneurship', 'Cybersecurity']</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>arXiv:2310.03736, arXiv:2310.03702, arXiv:2310.03655, arXiv:2310.03528, arXiv:2310.03501, arXiv:2310.03475, arXiv:2310.03441, arXiv:2310.03178, arXiv:2310.03159, arXiv:2310.03105</t>
-        </is>
-      </c>
+      <c r="D23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -955,11 +861,7 @@
           <t>['Computer Science', 'Education &amp; Educational Research', 'Software Engineering', 'Linguistics', 'Mathematics']</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>arXiv:2310.03736, arXiv:2310.03702, arXiv:2310.03655, arXiv:2310.03528, arXiv:2310.03501, arXiv:2310.03475, arXiv:2310.03441, arXiv:2310.03178, arXiv:2310.03159, arXiv:2310.03105</t>
-        </is>
-      </c>
+      <c r="D24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -977,11 +879,7 @@
           <t>['High performance computing', 'Computer systems architecture', 'Automatic differentiation', 'Distributed computing', 'Parallel computing', 'GPU computing', 'Numerical optimization algorithms', 'Computer modelling and simulation', 'Artificial Intelligence', 'Deep learning', 'Deep Neural Networks', 'Computer Vision', 'Embedded Systems', 'Efficient and scalable parallel algorithms', 'Scientific computing', 'scientific writing', 'Higher education', 'Online courses', 'Domenii ERC 2019', 'Supercomputing']</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>arXiv:2310.02422, arXiv:2311.02840, arXiv:2310.06916, arXiv:2310.04837, arXiv:2310.03294, arXiv:2310.00627, arXiv:2309.16743, arXiv:2310.08401, arXiv:2310.08097, arXiv:2310.07471</t>
-        </is>
-      </c>
+      <c r="D25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -999,11 +897,7 @@
           <t>['Computer Science', 'Software Engineering']</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>arXiv:2310.03736, arXiv:2310.03702, arXiv:2310.03655, arXiv:2310.03528, arXiv:2310.03501, arXiv:2310.03475, arXiv:2310.03441, arXiv:2310.03178, arXiv:2310.03159, arXiv:2310.03105</t>
-        </is>
-      </c>
+      <c r="D26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1021,11 +915,7 @@
           <t>['Automation &amp; Control Systems', 'Software Engineering', 'Computer Science', 'Robotics', 'Operations Research &amp; Management Science', 'Diagnosis and fault tolerant control', 'Mixed integer programming', 'Model predictive control', 'Unmanned vehicle systems']</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>arXiv:2310.01039, arXiv:2310.05170, arXiv:2310.15887, arXiv:2311.04569, arXiv:2311.04126, arXiv:2310.00029, arXiv:2311.02389, arXiv:2310.03673, arXiv:2310.03659, arXiv:2310.03620</t>
-        </is>
-      </c>
+      <c r="D27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1043,11 +933,7 @@
           <t>['Computer systems architecture', 'Computer networks', 'Embedded systems', 'Microprocessor systems', 'Distributed systems', 'Internet', 'Mobile computing', 'E-learning', 'Web platforms']</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>arXiv:2310.16214, arXiv:2311.03373, arXiv:2310.04172, arXiv:2311.05063, arXiv:2310.03618, arXiv:2310.03616, arXiv:2310.03568, arXiv:2310.03371, arXiv:2310.03294, arXiv:2310.03200</t>
-        </is>
-      </c>
+      <c r="D28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1065,11 +951,7 @@
           <t>['Business &amp; Economics', 'Software Engineering', 'Social Sciences - Other Topics', 'Automation &amp; Control Systems', 'Education &amp; Educational Research']</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>arXiv:2310.03673, arXiv:2310.03659, arXiv:2310.03620, arXiv:2310.03618, arXiv:2310.03616, arXiv:2310.03533, arXiv:2310.03491, arXiv:2310.03318, arXiv:2310.03248, arXiv:2310.03202</t>
-        </is>
-      </c>
+      <c r="D29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1087,11 +969,7 @@
           <t>['Databases', 'Data mining', 'Machine learning', 'Text mining']</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>arXiv:2310.05020, arXiv:2310.02540, arXiv:2310.02129, arXiv:2310.01765, arXiv:2310.00749, arXiv:2310.07875, arXiv:2310.07736, arXiv:2310.04830, arXiv:2310.04598, arXiv:2310.04145</t>
-        </is>
-      </c>
+      <c r="D30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1109,11 +987,7 @@
           <t>['Computer Science', 'Software Engineering', 'Automation &amp; Control Systems', 'Telecommunications', 'Instruments &amp; Instrumentation']</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>arXiv:2310.03736, arXiv:2310.03702, arXiv:2310.03655, arXiv:2310.03528, arXiv:2310.03501, arXiv:2310.03475, arXiv:2310.03441, arXiv:2310.03178, arXiv:2310.03159, arXiv:2310.03105</t>
-        </is>
-      </c>
+      <c r="D31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1131,11 +1005,7 @@
           <t>['Computer Science', 'Education &amp; Educational Research', 'Software Engineering', 'Energy &amp; Fuels', 'Automation &amp; Control Systems']</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>arXiv:2310.03736, arXiv:2310.03702, arXiv:2310.03655, arXiv:2310.03528, arXiv:2310.03501, arXiv:2310.03475, arXiv:2310.03441, arXiv:2310.03178, arXiv:2310.03159, arXiv:2310.03105</t>
-        </is>
-      </c>
+      <c r="D32" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added random generated rec + work on hybrid + small changes overall
</commit_message>
<xml_diff>
--- a/datasets/users/researchers.xlsx
+++ b/datasets/users/researchers.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -425,6 +425,7 @@
     <col width="30" customWidth="1" min="2" max="2"/>
     <col width="507" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -448,6 +449,11 @@
           <t>Appreciated</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Random Recommendation</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -822,7 +828,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>['Mobile communications', 'Wireless networks', 'Security and privacy in communications', 'Internet of Thingd', 'Radio propagation', 'Wearable computing', 'Energy meter', 'Wearable devices']</t>
+          <t>['Mobile communications', 'Wireless networks', 'Security and privacy in communications', 'Internet of Things', 'Radio propagation', 'Wearable computing', 'Energy meter', 'Wearable devices']</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>

</xml_diff>